<commit_message>
Added full ncdump of GOES16 test raw data file. Updated the Excel file to include comparison to a sample SEVIRI_m11 obs file. Updated paths in shell scripts.
</commit_message>
<xml_diff>
--- a/src/goes/notes/goes16_fields.xlsx
+++ b/src/goes/notes/goes16_fields.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric2/PROJECTS/IODA_CONVERTERS/ioda-converters/src/goes16/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eric2/PROJECTS/IODA_CONVERTERS/ioda-converters/src/goes/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE526C-BA32-D94B-9BD6-2BB1FC67677A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DC0AAA-252F-0E4D-8D80-7806A6D9C578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" xr2:uid="{537B1580-5777-7F46-8F25-390BC366EED8}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" activeTab="1" xr2:uid="{537B1580-5777-7F46-8F25-390BC366EED8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw Data Fields" sheetId="1" r:id="rId1"/>
+    <sheet name="Groups and Datasets" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="81">
   <si>
     <t>Field (short name)</t>
   </si>
@@ -196,6 +197,87 @@
   </si>
   <si>
     <t>IODAv2 Variable</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>EffectiveError</t>
+  </si>
+  <si>
+    <t>EffectiveQC</t>
+  </si>
+  <si>
+    <t>MetaData</t>
+  </si>
+  <si>
+    <t>ObsBias</t>
+  </si>
+  <si>
+    <t>ObsError</t>
+  </si>
+  <si>
+    <t>ObsValue</t>
+  </si>
+  <si>
+    <t>PreQC</t>
+  </si>
+  <si>
+    <t>VarMetaData</t>
+  </si>
+  <si>
+    <t>constantPredictor</t>
+  </si>
+  <si>
+    <t>emissivityPredictor</t>
+  </si>
+  <si>
+    <t>lapse_ratePredictor</t>
+  </si>
+  <si>
+    <t>lapse_rate_order_2Predictor</t>
+  </si>
+  <si>
+    <t>scan_anglePredictor</t>
+  </si>
+  <si>
+    <t>scan_angle_order_2Predictor</t>
+  </si>
+  <si>
+    <t>scan_angle_order_3Predictor</t>
+  </si>
+  <si>
+    <t>scan_angle_order_4Predictor</t>
+  </si>
+  <si>
+    <t>Root</t>
+  </si>
+  <si>
+    <t>nchans, ndatetime, nlocs, nstring, nvars</t>
+  </si>
+  <si>
+    <t>brightness_temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datetime, height_above_mean_sea_level, latitude, longitude, record_number, scan_position, sensor_azimuth_angle, sensor_view_angle, sensor_zenith_angle, solar_azimuth_angle, solar_zenith_angle, time </t>
+  </si>
+  <si>
+    <t>Datasets (SEVIRI_m11)</t>
+  </si>
+  <si>
+    <t>ObsError, mean_lapse_rate, polarization, sensor_band_central_radiation_frequency, sensor_band_central_radiation_wavenumber, sensor_channel, variable_names</t>
+  </si>
+  <si>
+    <t>Datasets ported from IODAv1 converter(GOES-16)</t>
+  </si>
+  <si>
+    <t>nlocs, nobs, nrecs, nvars</t>
+  </si>
+  <si>
+    <t>Elevation_Angle, Scan_Angle, latitude, longitude, time</t>
+  </si>
+  <si>
+    <t>radiance</t>
   </si>
 </sst>
 </file>
@@ -227,7 +309,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -308,11 +390,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +447,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8150D10-C533-E842-BCAE-057D83DF7627}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="144" zoomScaleNormal="144" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -935,4 +1061,198 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80BF457B-0C23-8844-AE0F-2A4B9A32ECD1}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.83203125" customWidth="1"/>
+    <col min="2" max="2" width="49.6640625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="50.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="89" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>